<commit_message>
Actualización de Sprints Semanales
Se agregaron los siguiente sprint al día, los cuales los teníamos en una carpeta de drive.
* Burdown Chart
* Daily Meeting
* Impediment Log
* Release
* Retrospective
* Review
* Scrumboard
* Sprint Backlogs
* Sprint Planning
</commit_message>
<xml_diff>
--- a/Sprints/Release/Documento Release – Proyecto APT.xlsx
+++ b/Sprints/Release/Documento Release – Proyecto APT.xlsx
@@ -81,7 +81,7 @@
     <t>Release 1.2 – Diseño y Arquitectura de Software</t>
   </si>
   <si>
-    <t>22 de septiembre – 15 de octubre 2025</t>
+    <t>22 de septiembre – 24 de octubre 2025</t>
   </si>
   <si>
     <t>- Diseño y documentación del modelo entidad-relación (ERD).
@@ -89,6 +89,9 @@
 - Creación de diagramas técnicos y documentación de respaldo.</t>
   </si>
   <si>
+    <t>En curso</t>
+  </si>
+  <si>
     <t>Se realizaron ajustes menores agregando columnas necesarias en algunas tablas.</t>
   </si>
   <si>
@@ -104,9 +107,6 @@
   </si>
   <si>
     <t>Gabriel Verdejo, Jonathan Gaete, Gonzalo Monreal</t>
-  </si>
-  <si>
-    <t>En curso</t>
   </si>
   <si>
     <t>El diseño del panel de publicaciones se ajustó al formato más dinámico y moderno. Se optimiza el rendimiento visual.</t>
@@ -133,7 +133,7 @@
     <t>11 de agosto – 29 de noviembre 2025</t>
   </si>
   <si>
-    <t>- Registro constante en GitHub y Trello.
+    <t>- Registro constante en GitHub.
 - Seguimiento de Sprints, reuniones y control de versiones.
 - Documentación de cambios y evidencias.</t>
   </si>
@@ -272,7 +272,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font/>
       <fill>
@@ -310,13 +310,29 @@
       </fill>
       <border/>
     </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF356854"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF356854"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF356854"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF356854"/>
+        </bottom>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="1">
     <tableStyle count="4" pivot="0" name="Hoja 1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
-      <tableStyleElement size="0" type="wholeTable"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -657,27 +673,27 @@
         <v>11</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>28</v>
@@ -697,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>32</v>
@@ -737,7 +753,7 @@
         <v>41</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>42</v>

</xml_diff>